<commit_message>
almost all constraints autotomatic
</commit_message>
<xml_diff>
--- a/output/df_conect.xlsx
+++ b/output/df_conect.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4F17CD-454F-4E2B-8361-AFCC70252447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2783D30A-A031-4664-A01F-A1CB6E6E2A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,15 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -464,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -482,7 +482,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -499,8 +499,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="O10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>